<commit_message>
test of null/none cases in OwcContext https://github.com/ZGIS/nz-gw-hub/issues/2
</commit_message>
<xml_diff>
--- a/test/resources/sparql/ResearchPrgrm.xlsx
+++ b/test/resources/sparql/ResearchPrgrm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>p.white@gns.cri.nz</t>
   </si>
@@ -65,134 +65,149 @@
     <t>This programme started in July 2016 and aims to improve national-scale hydrological knowledge access the New Zealand landscape with a combination of data on surface water, soil, geology and groundwater. The expected project duration is five to seven years. Case studies areas includes catchments located in the Gisborne, Horizons and Southland regions. This collaborative programme brings together the National Institute for Water and Atmospheric Research (NIWA, lead), Landcare Research and GNS Science. GNS Science will further develop their models of groundwater flow, groundwater age, and hydraulic properties of the subsurface.</t>
   </si>
   <si>
+    <t xml:space="preserve">National Hydrology Programme </t>
+  </si>
+  <si>
+    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/Smart-Models-for-Aquifer-Management-SAM</t>
+  </si>
+  <si>
+    <t>c.moore@gns.cri.nz</t>
+  </si>
+  <si>
+    <t>Catherine Moore</t>
+  </si>
+  <si>
+    <t>MBIE (Contestable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This project started in October 2015 and develops effective and streamlined groundwater surface water flow and transport models.  These models address problems at large-scales (catchment or region wide) and local scales (a local well or spring).  The project also provides methods for identifying optimal data acquisition efforts for these multi-scale predictions. The resulting models are suitable for quantification of uncertainty and run sufficiently quickly to support a comprehensive risk-based evaluation of design or policy alternatives.   These models can be rapidly built and therefore cost less to deploy than is the current norm; thus providing more widespread model based support for any model budget. </t>
+  </si>
+  <si>
+    <t>Smart Models for Aquifer Managements</t>
+  </si>
+  <si>
+    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/SMART-Aquifer-Characterisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.cameron@gns.cri.nz. </t>
+  </si>
+  <si>
+    <t>Stewart Cameron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This programme aimed to develop a suite of highly innovative methods for characterising New Zealand’s groundwater systems faster and/or less expensively than using traditional methods. This programme began in 2011 and ended in September 2017. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smart Aquifer Characterisation </t>
+  </si>
+  <si>
+    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/Groundwater-Resources-of-New-Zealand-GWR</t>
+  </si>
+  <si>
+    <t>m.moreau@gns.cri.nz</t>
+  </si>
+  <si>
+    <t>MBIE (SSIF-Infrastructure)</t>
+  </si>
+  <si>
+    <t>This research and monitoring programme is operated by GNS Science in collaboration with all of NZ regional authorities since 1998. It provides a national perspective on groundwater monitoring used to define “baseline” groundwater quality; associates groundwater quality with certain causes such as anthropogenic influence, and best-practice methods for sampling and monitoring as well as groundwater quality data interpretation.</t>
+  </si>
+  <si>
+    <t>National Groundwater Monitoring Programme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNS Science’s hydrogeology research programme, which is funded by MBIE Sustainable Science Investment Fund (2017-2024). The primary aim of the programme is to inform ways to improve the sustainable management of, and economic returns from groundwater resources in New Zealand. The programme objectives are to: understand the hydrogeological and structural characteristics of New Zealand’s aquifers; determine fluxes of water and key substances in, through, and out of these aquifers; develop and apply isotopic tools and biogeochemical tracers; determine impacts of pressures (e.g., human activities and climate change) on groundwater resources; and to assist stakeholders to improve social, cultural, environmental and economic outcomes. </t>
+  </si>
+  <si>
+    <t>Groundwater Resources of New Zealand</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Funding source</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Abreviation</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>GNS Science</t>
+  </si>
+  <si>
+    <t>Organisation (lead)</t>
+  </si>
+  <si>
+    <t>Rogier Westerhoff</t>
+  </si>
+  <si>
+    <t>Magali Moreau</t>
+  </si>
+  <si>
+    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes</t>
+  </si>
+  <si>
+    <t>Mailto (hidden)</t>
+  </si>
+  <si>
+    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/National-Groundwater-Monitoring-Programme-NGMP</t>
+  </si>
+  <si>
+    <t>Ka Tu Te Taniwha – Ka Ora Te Tangata</t>
+  </si>
+  <si>
+    <t>https://gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/Past-research-programmes/Ka-Tu-Te-Taniwha-Ka-Ora-Te-Tangata</t>
+  </si>
+  <si>
+    <t>This collaborative project (2014-2016) aimed to understand the impacts of development in the Awahou groundwater catchment to ensure the health and wellbeing of the Ngati Rangiwewehi people. The project output is an integrated data repository and knowledge resource, which combined technical, scientific and Mātauranga-a-iwi information for the Awahou groundwater catchment. This allowed Ngāti Rangiwewehi to incorporate traditional knowledge and understanding of cultural significance to inform and plan for future freshwater development in the Awahou catchment.</t>
+  </si>
+  <si>
+    <t>Te Pūnaha Hihiko - Vision Mātauranga Connect Scheme; Ngati Rangiwewehi; Bay of Plenty Regional Council.</t>
+  </si>
+  <si>
+    <t>Conny Tschritter</t>
+  </si>
+  <si>
+    <t>c.tschritter@gns.cri.nz</t>
+  </si>
+  <si>
+    <t>GWR</t>
+  </si>
+  <si>
+    <t>NGMP</t>
+  </si>
+  <si>
+    <t>SAC</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
     <t>NHP</t>
   </si>
   <si>
-    <t xml:space="preserve">National Hydrology Programme </t>
-  </si>
-  <si>
-    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/Smart-Models-for-Aquifer-Management-SAM</t>
-  </si>
-  <si>
-    <t>c.moore@gns.cri.nz</t>
-  </si>
-  <si>
-    <t>Catherine Moore</t>
-  </si>
-  <si>
-    <t>MBIE (Contestable)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This project started in October 2015 and develops effective and streamlined groundwater surface water flow and transport models.  These models address problems at large-scales (catchment or region wide) and local scales (a local well or spring).  The project also provides methods for identifying optimal data acquisition efforts for these multi-scale predictions. The resulting models are suitable for quantification of uncertainty and run sufficiently quickly to support a comprehensive risk-based evaluation of design or policy alternatives.   These models can be rapidly built and therefore cost less to deploy than is the current norm; thus providing more widespread model based support for any model budget. </t>
-  </si>
-  <si>
-    <t>SAM</t>
-  </si>
-  <si>
-    <t>Smart Models for Aquifer Managements</t>
-  </si>
-  <si>
-    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/SMART-Aquifer-Characterisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s.cameron@gns.cri.nz. </t>
-  </si>
-  <si>
-    <t>Stewart Cameron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This programme aimed to develop a suite of highly innovative methods for characterising New Zealand’s groundwater systems faster and/or less expensively than using traditional methods. This programme began in 2011 and ended in September 2017. </t>
-  </si>
-  <si>
-    <t>SAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smart Aquifer Characterisation </t>
-  </si>
-  <si>
-    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/Groundwater-Resources-of-New-Zealand-GWR</t>
-  </si>
-  <si>
-    <t>m.moreau@gns.cri.nz</t>
-  </si>
-  <si>
-    <t>MBIE (SSIF-Infrastructure)</t>
-  </si>
-  <si>
-    <t>This research and monitoring programme is operated by GNS Science in collaboration with all of NZ regional authorities since 1998. It provides a national perspective on groundwater monitoring used to define “baseline” groundwater quality; associates groundwater quality with certain causes such as anthropogenic influence, and best-practice methods for sampling and monitoring as well as groundwater quality data interpretation.</t>
-  </si>
-  <si>
-    <t>NGMP</t>
-  </si>
-  <si>
-    <t>National Groundwater Monitoring Programme</t>
-  </si>
-  <si>
-    <t>Abigail Lovett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GNS Science’s hydrogeology research programme, which is funded by MBIE Sustainable Science Investment Fund (2017-2024). The primary aim of the programme is to inform ways to improve the sustainable management of, and economic returns from groundwater resources in New Zealand. The programme objectives are to: understand the hydrogeological and structural characteristics of New Zealand’s aquifers; determine fluxes of water and key substances in, through, and out of these aquifers; develop and apply isotopic tools and biogeochemical tracers; determine impacts of pressures (e.g., human activities and climate change) on groundwater resources; and to assist stakeholders to improve social, cultural, environmental and economic outcomes. </t>
-  </si>
-  <si>
-    <t>GWR</t>
-  </si>
-  <si>
-    <t>Groundwater Resources of New Zealand</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Funding source</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Abreviation</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>GNS Science</t>
-  </si>
-  <si>
-    <t>Organisation (lead)</t>
-  </si>
-  <si>
-    <t>Rogier Westerhoff</t>
-  </si>
-  <si>
-    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes/Groundwater-Resources-of-New-Zealand-GWR/The-National-Groundwater-Monitoring-Programme-NGMP</t>
-  </si>
-  <si>
-    <t>a.lovett@gns.cri.nz</t>
-  </si>
-  <si>
-    <t>Magali Moreau</t>
-  </si>
-  <si>
-    <t>https://www.gns.cri.nz/Home/Our-Science/Environment-and-Materials/Groundwater/Research-Programmes</t>
-  </si>
-  <si>
-    <t>VM-Piako</t>
-  </si>
-  <si>
-    <t>VM-Awahou-Kaitiaki</t>
-  </si>
-  <si>
-    <t>Mailto (hidden)</t>
+    <t>VM-PIAKO</t>
+  </si>
+  <si>
+    <t>VM-Kaitiaki</t>
+  </si>
+  <si>
+    <t>VM-Awahou</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,12 +233,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -256,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -264,13 +273,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -589,179 +606,183 @@
   <dimension ref="A1:H1048572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="17.265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="79.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" style="1"/>
+    <col min="5" max="5" width="22.3984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
+      <c r="H1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="122.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="81.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
+    </row>
+    <row r="4" spans="1:8" ht="41.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="122.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="H5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="108.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="H6" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="122.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -771,23 +792,23 @@
         <v>6</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="H7" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="81.75" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -797,13 +818,39 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>50</v>
+      <c r="H8" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="95.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="1048572" spans="6:6" x14ac:dyDescent="0.45">
@@ -818,15 +865,16 @@
     <hyperlink ref="G7" r:id="rId5" display="mailto:z.rawlinson@gns.cri.nz"/>
     <hyperlink ref="G6" r:id="rId6" display="mailto:r.westerhoff@gns.cri.nz"/>
     <hyperlink ref="H2" r:id="rId7"/>
-    <hyperlink ref="H3" r:id="rId8"/>
-    <hyperlink ref="H4" r:id="rId9"/>
-    <hyperlink ref="H5" r:id="rId10"/>
-    <hyperlink ref="G2" r:id="rId11"/>
-    <hyperlink ref="H6" r:id="rId12"/>
-    <hyperlink ref="H7" r:id="rId13"/>
-    <hyperlink ref="H8" r:id="rId14"/>
+    <hyperlink ref="H4" r:id="rId8"/>
+    <hyperlink ref="H5" r:id="rId9"/>
+    <hyperlink ref="G2" r:id="rId10"/>
+    <hyperlink ref="H6" r:id="rId11"/>
+    <hyperlink ref="H7" r:id="rId12"/>
+    <hyperlink ref="H8" r:id="rId13"/>
+    <hyperlink ref="G9" r:id="rId14" display="mailto:p.white@gns.cri.nz"/>
+    <hyperlink ref="H9" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>